<commit_message>
Arreglo bug de las letras
</commit_message>
<xml_diff>
--- a/Rogue-Lite/Assets/Game/Resources/Menus/Menus.xlsx
+++ b/Rogue-Lite/Assets/Game/Resources/Menus/Menus.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="186">
   <si>
     <t>Index</t>
   </si>
@@ -429,49 +429,151 @@
     <t>Presiona</t>
   </si>
   <si>
+    <t>Drücken</t>
+  </si>
+  <si>
     <t>to walk</t>
   </si>
   <si>
     <t>para andar</t>
   </si>
   <si>
+    <t>um tu gehen</t>
+  </si>
+  <si>
     <t>Left click to attack</t>
   </si>
   <si>
     <t>Click izquierdo para atacar</t>
   </si>
   <si>
+    <t>Linksklick zum Angriff</t>
+  </si>
+  <si>
     <t>Right click for special skill</t>
   </si>
   <si>
     <t>Click derecho para la habilidad especial</t>
   </si>
   <si>
+    <t>Rechtsclick für besondere Fähigkeit</t>
+  </si>
+  <si>
     <t>Press SPACEBAR to roll</t>
   </si>
   <si>
     <t>Presiona ESPACIO para rodar</t>
   </si>
   <si>
+    <t>LEERTASTE zum rollen</t>
+  </si>
+  <si>
     <t>Health</t>
   </si>
   <si>
     <t>Salud</t>
   </si>
   <si>
+    <t>Leben</t>
+  </si>
+  <si>
     <t>Strength</t>
   </si>
   <si>
     <t>Fuerza</t>
   </si>
   <si>
+    <t>Stärke</t>
+  </si>
+  <si>
     <t>Dungeon Level</t>
   </si>
   <si>
     <t>Nivel de Mazmorra</t>
   </si>
   <si>
+    <t>Kerkerniveau</t>
+  </si>
+  <si>
+    <t>Purchase upgrade</t>
+  </si>
+  <si>
     <t>Pagar mejora</t>
+  </si>
+  <si>
+    <t>Upgrade kaufen</t>
+  </si>
+  <si>
+    <t>Bladesmith</t>
+  </si>
+  <si>
+    <t>Armero</t>
+  </si>
+  <si>
+    <t>Waffenschmid</t>
+  </si>
+  <si>
+    <t>Blacksmith</t>
+  </si>
+  <si>
+    <t>Herrero</t>
+  </si>
+  <si>
+    <t>Schmied</t>
+  </si>
+  <si>
+    <t>Dyer</t>
+  </si>
+  <si>
+    <t>Hombre de la tintonería</t>
+  </si>
+  <si>
+    <t>Färber</t>
+  </si>
+  <si>
+    <t>Magician</t>
+  </si>
+  <si>
+    <t>Maga</t>
+  </si>
+  <si>
+    <t>Zauberin</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Coste</t>
+  </si>
+  <si>
+    <t>Kosten</t>
+  </si>
+  <si>
+    <t>Press any key to continue</t>
+  </si>
+  <si>
+    <t>Presiona cualquier tecla para continuar</t>
+  </si>
+  <si>
+    <t>Um zu starten beliebige Taste drücken</t>
+  </si>
+  <si>
+    <t>Tap the screen to continue</t>
+  </si>
+  <si>
+    <t>Pulsa la pantalla para continuar</t>
+  </si>
+  <si>
+    <t>Tippen Sie auf den Bildschirm</t>
+  </si>
+  <si>
+    <t>Modify</t>
+  </si>
+  <si>
+    <t>Modificar</t>
+  </si>
+  <si>
+    <t>Modifizieren</t>
   </si>
 </sst>
 </file>
@@ -516,7 +618,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -531,9 +633,6 @@
     </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1227,7 +1326,9 @@
       <c r="B34" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C34" s="5"/>
+      <c r="C34" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="D34" s="4" t="s">
         <v>94</v>
       </c>
@@ -1466,110 +1567,234 @@
       <c r="C51" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="D51" s="4"/>
+      <c r="D51" s="4" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="3">
         <v>50.0</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D52" s="4"/>
+        <v>139</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="3">
         <v>51.0</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="D53" s="4"/>
+        <v>142</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="3">
         <v>52.0</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D54" s="4"/>
+        <v>145</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="3">
         <v>53.0</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="D55" s="4"/>
+        <v>148</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="3">
         <v>54.0</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D56" s="4"/>
+        <v>151</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="3">
         <v>55.0</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="D57" s="4"/>
+        <v>154</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="3">
         <v>56.0</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="D58" s="4"/>
+        <v>157</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="3">
         <v>57.0</v>
       </c>
-      <c r="B59" s="4"/>
+      <c r="B59" s="4" t="s">
+        <v>159</v>
+      </c>
       <c r="C59" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="D59" s="4"/>
-    </row>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
-    <row r="62" ht="15.75" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
-    <row r="64" ht="15.75" customHeight="1"/>
-    <row r="65" ht="15.75" customHeight="1"/>
-    <row r="66" ht="15.75" customHeight="1"/>
-    <row r="67" ht="15.75" customHeight="1"/>
+        <v>160</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="60" ht="15.75" customHeight="1">
+      <c r="A60" s="3">
+        <v>58.0</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="61" ht="15.75" customHeight="1">
+      <c r="A61" s="3">
+        <v>59.0</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="62" ht="15.75" customHeight="1">
+      <c r="A62" s="3">
+        <v>60.0</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="63" ht="15.75" customHeight="1">
+      <c r="A63" s="3">
+        <v>61.0</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="64" ht="15.75" customHeight="1">
+      <c r="A64" s="3">
+        <v>62.0</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="65" ht="15.75" customHeight="1">
+      <c r="A65" s="3">
+        <v>63.0</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="66" ht="15.75" customHeight="1">
+      <c r="A66" s="3">
+        <v>64.0</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="67" ht="15.75" customHeight="1">
+      <c r="A67" s="3">
+        <v>65.0</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
     <row r="68" ht="15.75" customHeight="1"/>
     <row r="69" ht="15.75" customHeight="1"/>
     <row r="70" ht="15.75" customHeight="1"/>

</xml_diff>